<commit_message>
formatting food from forest fig
</commit_message>
<xml_diff>
--- a/data/Foods_From_Forests_data/Copy of Southeast harvest summary_mg.xlsx
+++ b/data/Foods_From_Forests_data/Copy of Southeast harvest summary_mg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariegutgesell/Desktop/Wild Foods Repo/data/Foods_From_Forests_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917BD3FF-D7AF-734C-8FA3-09F7645F85D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C04CA2-9B3C-1946-A291-A05F5187B4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="21140" windowHeight="16480" activeTab="6" xr2:uid="{31312463-82D5-4964-87E9-66FCD054679B}"/>
   </bookViews>
@@ -4969,10 +4969,13 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
updates to excel categories
</commit_message>
<xml_diff>
--- a/data/Foods_From_Forests_data/Copy of Southeast harvest summary_mg.xlsx
+++ b/data/Foods_From_Forests_data/Copy of Southeast harvest summary_mg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariegutgesell/Desktop/Wild Foods Repo/data/Foods_From_Forests_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D903AB78-2885-7A49-8C76-E946FF10FE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8749AE2-C962-0D46-B822-46293B50EFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33400" yWindow="500" windowWidth="32400" windowHeight="20060" activeTab="7" xr2:uid="{31312463-82D5-4964-87E9-66FCD054679B}"/>
+    <workbookView xWindow="5560" yWindow="620" windowWidth="23240" windowHeight="16480" activeTab="7" xr2:uid="{31312463-82D5-4964-87E9-66FCD054679B}"/>
   </bookViews>
   <sheets>
     <sheet name="Anadromous" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Full_Sp_List!$A$1:$H$1152</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Resource_List!$A$1:$J$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -11316,7 +11317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA01B77-1536-4C70-86D4-A1F20DBA7FD4}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
@@ -32392,13 +32393,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B98C8E8-8A1F-7B41-A4C8-235CE5DB550D}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="34.5" customWidth="1"/>
     <col min="12" max="12" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -33153,6 +33155,7 @@
       <c r="C54" s="19"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J54" xr:uid="{3B98C8E8-8A1F-7B41-A4C8-235CE5DB550D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C41">
     <sortCondition ref="A2:A41"/>
     <sortCondition ref="C2:C41"/>

</xml_diff>